<commit_message>
Finalized code by adding function and chart
</commit_message>
<xml_diff>
--- a/spreadsheet_automation/transactions.xlsx
+++ b/spreadsheet_automation/transactions.xlsx
@@ -22,6 +22,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -68,7 +69,10 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -92,6 +96,135 @@
     <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>New corrected price chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>New Price</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Y-Axis</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -386,70 +519,76 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+      <selection activeCell="D1" activeCellId="0" pane="topLeft" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="11.52"/>
+    <col customWidth="1" max="1023" min="1" style="3" width="11.52"/>
+    <col customWidth="1" max="1025" min="1024" style="3" width="11.52"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>transaction_id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>product_id</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">price </t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Corrected Price</t>
+        </is>
+      </c>
     </row>
-    <row customHeight="1" ht="12.8" r="2" s="3">
-      <c r="A2" s="2" t="n">
+    <row customHeight="1" ht="12.8" r="2" s="4">
+      <c r="A2" s="3" t="n">
         <v>1001</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="5" t="n">
         <v>5.95</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" t="n">
         <v>5.355</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="3" s="3">
-      <c r="A3" s="2" t="n">
+    <row customHeight="1" ht="12.8" r="3" s="4">
+      <c r="A3" s="3" t="n">
         <v>1002</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>6.95</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" t="n">
         <v>6.255</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="4" s="3">
-      <c r="A4" s="2" t="n">
+    <row customHeight="1" ht="12.8" r="4" s="4">
+      <c r="A4" s="3" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>7.95</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" t="n">
         <v>7.155</v>
       </c>
     </row>
@@ -465,5 +604,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>